<commit_message>
Excel media file updated.
</commit_message>
<xml_diff>
--- a/dev/0.1_Description_4_media_key_messages_&_captions/1.0_key_messages_&_captions.xlsx
+++ b/dev/0.1_Description_4_media_key_messages_&_captions/1.0_key_messages_&_captions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sicaja\Desktop\SmartCodeACADEMY\0.0_Channel_topics\2025.03.22-GitHub_AI_Marketing_Generator\dev\0.1_Description_4_media_key_messages_&amp;_captions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170AD122-913D-46A9-B43E-41A8105EED76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CBC5ED-DCB9-4B39-9E6A-304C3ABBB58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -260,9 +260,6 @@
     <t>Output</t>
   </si>
   <si>
-    <t>C:\Users\Sicaja\Desktop\SmartCodeACADEMY\0.0_Channel_topics\2025.03.22-GitHub_AI_Marketing_Generator\0.1_GitHub</t>
-  </si>
-  <si>
     <t>Add key messages, captions, and product DB; update app.py  model  to Mistral and added template of the  README</t>
   </si>
   <si>
@@ -423,6 +420,9 @@
   </si>
   <si>
     <t>ai created - conceptual</t>
+  </si>
+  <si>
+    <t>C:\Users\Sicaja\Desktop\SmartCodeACADEMY\0.0_Channel_topics\2025.03.22-GitHub_AI_Marketing_Generator</t>
   </si>
 </sst>
 </file>
@@ -997,7 +997,7 @@
         <v>61</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1042,10 +1042,10 @@
     </row>
     <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="C14" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1117,7 +1117,7 @@
         <v>49</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
@@ -1227,92 +1227,92 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -1322,148 +1322,148 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s">
         <v>87</v>
-      </c>
-      <c r="C27" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" t="s">
         <v>91</v>
-      </c>
-      <c r="C30" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1485,7 +1485,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,7 +1500,7 @@
         <v>62</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1509,12 +1509,12 @@
       </c>
       <c r="B2" s="6" t="str">
         <f>SUBSTITUTE(B1, "\", "/")</f>
-        <v>C:/Users/Sicaja/Desktop/SmartCodeACADEMY/0.0_Channel_topics/2025.03.22-GitHub_AI_Marketing_Generator/0.1_GitHub</v>
+        <v>C:/Users/Sicaja/Desktop/SmartCodeACADEMY/0.0_Channel_topics/2025.03.22-GitHub_AI_Marketing_Generator</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scripts updated with Llama 3.1 8B Instruct model deployed as HF endpoint.
</commit_message>
<xml_diff>
--- a/dev/0.1_Description_4_media_key_messages_&_captions/1.0_key_messages_&_captions.xlsx
+++ b/dev/0.1_Description_4_media_key_messages_&_captions/1.0_key_messages_&_captions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sicaja\Desktop\SmartCodeACADEMY\0.0_Channel_topics\2025.03.22-GitHub_AI_Marketing_Generator\dev\0.1_Description_4_media_key_messages_&amp;_captions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7BF806-DFA5-47AC-BE6D-AAE78CA63B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8F75D8-5E08-4342-8EF5-E0BA6A155A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="key_messages_&amp;_captiosn" sheetId="2" r:id="rId1"/>
@@ -907,12 +907,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFA82D05-3B3C-41E0-860A-3A51304EF733}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,7 +1478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80838B4-7FF7-4A54-BF52-AC4F2521D054}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>